<commit_message>
content that has gone through testing, ready for prod
</commit_message>
<xml_diff>
--- a/src/Problem_Bank_URL.xlsx
+++ b/src/Problem_Bank_URL.xlsx
@@ -37,7 +37,7 @@
     <t>Under development</t>
   </si>
   <si>
-    <t>OpenStax PreAlgebra</t>
+    <t>PreAlgebra</t>
   </si>
   <si>
     <t>/Users/leyla/Projects/EdTech/WazaTutor-Content/src/PreAlgebra/WazaTutor_PreAlgebra.xlsx</t>
@@ -415,7 +415,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.63"/>
-    <col customWidth="1" min="2" max="2" width="45.38"/>
+    <col customWidth="1" min="2" max="2" width="54.88"/>
     <col customWidth="1" min="3" max="3" width="49.5"/>
     <col customWidth="1" min="4" max="4" width="16.0"/>
     <col customWidth="1" min="5" max="28" width="12.63"/>

</xml_diff>